<commit_message>
Added test_cases.xlsx Excel file
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/PA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnn\PycharmProjects\cs151-pa1-jpelehwany\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0D32F8-6D7A-7B45-9670-B8699C8948C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D06CAD9-5F3E-4EDE-8375-A0F56A097B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,16 +34,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>You need to create your own tests</t>
+  </si>
+  <si>
+    <t>Confident, Good Answers</t>
+  </si>
+  <si>
+    <t>Confident, Okay Answers</t>
+  </si>
+  <si>
+    <t>Confident, Bad Answers</t>
+  </si>
+  <si>
+    <t>Neutral, Good Answers</t>
+  </si>
+  <si>
+    <t>Confidence Level</t>
+  </si>
+  <si>
+    <t>MC 1 Points</t>
+  </si>
+  <si>
+    <t>DATA IN</t>
+  </si>
+  <si>
+    <t>Neutral, Okay Answers</t>
+  </si>
+  <si>
+    <t>Neutral, Bad Answers</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Uncofident, Good Answers</t>
+  </si>
+  <si>
+    <t>Uncofident, Okay Answers</t>
+  </si>
+  <si>
+    <t>Unconfident, Bad Answers</t>
+  </si>
+  <si>
+    <t>WR Points</t>
+  </si>
+  <si>
+    <t>Presentation Points</t>
+  </si>
+  <si>
+    <t>Confident Multiplier</t>
+  </si>
+  <si>
+    <t>Neutral Multiplier</t>
+  </si>
+  <si>
+    <t>Unconfident Multiplier</t>
+  </si>
+  <si>
+    <t>MC 2 Points</t>
+  </si>
+  <si>
+    <t>DATA OUT</t>
+  </si>
+  <si>
+    <t>Total Points</t>
+  </si>
+  <si>
+    <t>Pass or Fail</t>
+  </si>
+  <si>
+    <t>Required Points to Pass</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -51,13 +126,54 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,16 +185,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -95,9 +223,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,7 +263,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -241,7 +369,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,15 +519,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF6E1F2-B43E-D343-BB9B-DE90F40B65C5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.25" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="18.125" customWidth="1"/>
+    <col min="9" max="9" width="10.875" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="11" max="11" width="11.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,9 +545,336 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <f>5*C3</f>
+        <v>10.5</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <f>SUM(D12,E12,F12,G12)</f>
+        <v>30.5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f>5*C3</f>
+        <v>10.5</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I20" si="0">SUM(D13,E13,F13,G13)</f>
+        <v>22.5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <f>5*C3</f>
+        <v>10.5</v>
+      </c>
+      <c r="G14">
+        <v>-10</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f>3*C4</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>24.8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <f>3*C4</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>16.8</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f>3*C4</f>
+        <v>4.8000000000000007</v>
+      </c>
+      <c r="G17">
+        <v>-10</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>-3.1999999999999993</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <f>1*C5</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>21.1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f>1*C5</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>13.1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <f>1*C5</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G20">
+        <v>-10</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>-6.9</v>
+      </c>
+      <c r="J20" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>